<commit_message>
cambio de def a String
</commit_message>
<xml_diff>
--- a/ProjectsToPublish.xlsx
+++ b/ProjectsToPublish.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Jenkins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E205E15-2504-48A2-8809-2F2C3E01348D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439BF29B-3B11-4EB1-B306-40CF36C7172A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11505" xr2:uid="{232C2E75-DCBC-4924-AE5A-0A313BE6BAAE}"/>
   </bookViews>
@@ -34,21 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>AmxCoMovPosTemplates022_B27</t>
+    <t>Projects</t>
   </si>
   <si>
-    <t>AmxCoMovPosBasesFunBloq005_B27</t>
-  </si>
-  <si>
-    <t>AmxCoMovPosOptFunBloq006_B27</t>
-  </si>
-  <si>
-    <t>AmxCoMovPosOptDesc010_B27</t>
-  </si>
-  <si>
-    <t>Projects</t>
+    <t>TestProject001</t>
   </si>
 </sst>
 </file>
@@ -411,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1EBC66-685E-42AD-85C6-222DFBBC3ADD}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,27 +415,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agrega la publicacion
</commit_message>
<xml_diff>
--- a/ProjectsToPublish.xlsx
+++ b/ProjectsToPublish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Jenkins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631C3CA0-4B81-4AB3-969D-EC743C97D70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9E90C1-9051-4738-8F8D-585A02F98792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11505" xr2:uid="{232C2E75-DCBC-4924-AE5A-0A313BE6BAAE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{232C2E75-DCBC-4924-AE5A-0A313BE6BAAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Projects</t>
   </si>
   <si>
-    <t>TestProjectCoagus001</t>
+    <t>TestRuben</t>
+  </si>
+  <si>
+    <t>TestRuben1</t>
   </si>
 </sst>
 </file>
@@ -402,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1EBC66-685E-42AD-85C6-222DFBBC3ADD}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,6 +426,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>